<commit_message>
remove version from procedure requirements
</commit_message>
<xml_diff>
--- a/lib/onc_certification_g10_test_kit/requirements/(g)(10)-test-procedure_requirements.xlsx
+++ b/lib/onc_certification_g10_test_kit/requirements/(g)(10)-test-procedure_requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/onc-certification-g10-test-kit/lib/onc_certification_g10_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B61285-583B-5D4F-89CC-228872D2426C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A05D03-EF05-7A4C-80FD-04B7F5C04EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1040" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="880" yWindow="1040" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1572,12 +1572,6 @@
   </si>
   <si>
     <t>https://www.healthit.gov/test-method/standardized-api-patient-and-population-services#test_procedure</t>
-  </si>
-  <si>
-    <t>170.315(g)(10)-test-procedure_1.4</t>
-  </si>
-  <si>
-    <t>1.4</t>
   </si>
   <si>
     <t>SEC-CNN-1</t>
@@ -2429,6 +2423,12 @@
 * "ServiceRequest"
 The following resources must also be supported if using US Core 7.0.0 [([link](https://hl7.org/fhir/us/core/STU7/index.html))]:
 * "Location"</t>
+  </si>
+  <si>
+    <t>170.315(g)(10)-test-procedure</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -2885,6 +2885,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2903,7 +2904,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3274,14 +3274,14 @@
       <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="35"/>
       <c r="C5" s="30"/>
     </row>
@@ -3293,17 +3293,17 @@
       <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="41"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
@@ -3328,7 +3328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AJ78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -3372,7 +3372,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
@@ -3422,15 +3422,15 @@
       <c r="U1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:36" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>27</v>
@@ -3464,15 +3464,15 @@
       <c r="Z2" s="12"/>
       <c r="AD2" s="12"/>
     </row>
-    <row r="3" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>27</v>
@@ -3502,15 +3502,15 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
     </row>
-    <row r="4" spans="1:36" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>27</v>
@@ -3537,15 +3537,15 @@
       <c r="AE4" s="5"/>
       <c r="AF4" s="5"/>
     </row>
-    <row r="5" spans="1:36" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>27</v>
@@ -3572,15 +3572,15 @@
       <c r="AE5" s="5"/>
       <c r="AF5" s="5"/>
     </row>
-    <row r="6" spans="1:36" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>27</v>
@@ -3592,15 +3592,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>27</v>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="8" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>27</v>
@@ -3632,15 +3632,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>27</v>
@@ -3652,15 +3652,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>27</v>
@@ -3674,13 +3674,13 @@
     </row>
     <row r="11" spans="1:36" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>27</v>
@@ -3692,15 +3692,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="204" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="221" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>27</v>
@@ -3712,15 +3712,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>27</v>
@@ -3734,13 +3734,13 @@
     </row>
     <row r="14" spans="1:36" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>27</v>
@@ -3754,73 +3754,73 @@
     </row>
     <row r="15" spans="1:36" ht="187" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="323" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="272" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="B18" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>27</v>
@@ -3834,13 +3834,13 @@
     </row>
     <row r="19" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>27</v>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="20" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>27</v>
@@ -3874,13 +3874,13 @@
     </row>
     <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>27</v>
@@ -3892,15 +3892,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>27</v>
@@ -3912,15 +3912,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>27</v>
@@ -3932,15 +3932,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>27</v>
@@ -3954,13 +3954,13 @@
     </row>
     <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>27</v>
@@ -3974,13 +3974,13 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>27</v>
@@ -3992,15 +3992,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>27</v>
@@ -4014,13 +4014,13 @@
     </row>
     <row r="28" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>27</v>
@@ -4034,73 +4034,73 @@
     </row>
     <row r="29" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="B32" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>27</v>
@@ -4114,13 +4114,13 @@
     </row>
     <row r="33" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>27</v>
@@ -4134,13 +4134,13 @@
     </row>
     <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>27</v>
@@ -4154,13 +4154,13 @@
     </row>
     <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>27</v>
@@ -4174,13 +4174,13 @@
     </row>
     <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>27</v>
@@ -4192,15 +4192,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>27</v>
@@ -4214,13 +4214,13 @@
     </row>
     <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>27</v>
@@ -4234,13 +4234,13 @@
     </row>
     <row r="39" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>27</v>
@@ -4254,13 +4254,13 @@
     </row>
     <row r="40" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>27</v>
@@ -4274,13 +4274,13 @@
     </row>
     <row r="41" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>27</v>
@@ -4294,13 +4294,13 @@
     </row>
     <row r="42" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>27</v>
@@ -4314,13 +4314,13 @@
     </row>
     <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>27</v>
@@ -4334,13 +4334,13 @@
     </row>
     <row r="44" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>27</v>
@@ -4354,13 +4354,13 @@
     </row>
     <row r="45" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>27</v>
@@ -4374,13 +4374,13 @@
     </row>
     <row r="46" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>27</v>
@@ -4394,13 +4394,13 @@
     </row>
     <row r="47" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>27</v>
@@ -4414,13 +4414,13 @@
     </row>
     <row r="48" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>27</v>
@@ -4434,13 +4434,13 @@
     </row>
     <row r="49" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>27</v>
@@ -4454,13 +4454,13 @@
     </row>
     <row r="50" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>27</v>
@@ -4474,13 +4474,13 @@
     </row>
     <row r="51" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>27</v>
@@ -4494,13 +4494,13 @@
     </row>
     <row r="52" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>27</v>
@@ -4514,13 +4514,13 @@
     </row>
     <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>27</v>
@@ -4534,13 +4534,13 @@
     </row>
     <row r="54" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>27</v>
@@ -4554,13 +4554,13 @@
     </row>
     <row r="55" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>27</v>
@@ -4572,15 +4572,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>27</v>
@@ -4594,13 +4594,13 @@
     </row>
     <row r="57" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>27</v>
@@ -4614,13 +4614,13 @@
     </row>
     <row r="58" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>27</v>
@@ -4634,13 +4634,13 @@
     </row>
     <row r="59" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>27</v>
@@ -4654,13 +4654,13 @@
     </row>
     <row r="60" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>27</v>
@@ -4674,13 +4674,13 @@
     </row>
     <row r="61" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>27</v>
@@ -4694,13 +4694,13 @@
     </row>
     <row r="62" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>27</v>
@@ -4714,13 +4714,13 @@
     </row>
     <row r="63" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>27</v>
@@ -4734,13 +4734,13 @@
     </row>
     <row r="64" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>27</v>
@@ -4754,13 +4754,13 @@
     </row>
     <row r="65" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B65" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>27</v>
@@ -4774,13 +4774,13 @@
     </row>
     <row r="66" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>27</v>
@@ -4794,13 +4794,13 @@
     </row>
     <row r="67" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>27</v>
@@ -4814,13 +4814,13 @@
     </row>
     <row r="68" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>27</v>
@@ -4834,13 +4834,13 @@
     </row>
     <row r="69" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>27</v>
@@ -4854,13 +4854,13 @@
     </row>
     <row r="70" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>27</v>
@@ -4874,13 +4874,13 @@
     </row>
     <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>27</v>
@@ -4894,13 +4894,13 @@
     </row>
     <row r="72" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>27</v>
@@ -4914,13 +4914,13 @@
     </row>
     <row r="73" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>27</v>
@@ -4934,13 +4934,13 @@
     </row>
     <row r="74" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>27</v>
@@ -4954,13 +4954,13 @@
     </row>
     <row r="75" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>27</v>
@@ -4974,13 +4974,13 @@
     </row>
     <row r="76" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>27</v>
@@ -4994,13 +4994,13 @@
     </row>
     <row r="77" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>27</v>
@@ -5014,13 +5014,13 @@
     </row>
     <row r="78" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>27</v>
@@ -5074,8 +5074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5085,28 +5085,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="42"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>61</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="36" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>62</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -5300,12 +5300,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5563,22 +5567,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5604,19 +5614,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>